<commit_message>
Corregendo para nao peorer
</commit_message>
<xml_diff>
--- a/Normalizacao_Exercicios.xlsx
+++ b/Normalizacao_Exercicios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaio_mazza\Documents\GitHub\KaioMazza_BD_Exemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A757275-0967-419A-9291-47D625055953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E9224D-4802-40E4-95DA-5D67C676985A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD308EDE-B1E9-4E04-89A9-A5D1CED6390C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AD308EDE-B1E9-4E04-89A9-A5D1CED6390C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ex_01" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Nome</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>B Santos</t>
+  </si>
+  <si>
+    <t>Cod. Cliente (FK)</t>
+  </si>
+  <si>
+    <t>Cod. Telefone (PK)</t>
   </si>
 </sst>
 </file>
@@ -234,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -314,6 +320,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -325,7 +340,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,46 +348,45 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,10 +402,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Ênfase1" xfId="1" builtinId="31"/>
@@ -733,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6007966-AF76-4124-93A3-2251E5EDBEE5}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -749,78 +765,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="16"/>
       <c r="D1" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -828,14 +844,14 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>2</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -860,7 +876,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,32 +890,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -954,30 +970,30 @@
       <c r="F5" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="E7" s="21" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="E7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1055,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C4C5BC-9D70-465B-81BB-307ABD35048B}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,144 +1081,143 @@
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="16"/>
       <c r="D1" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="H1" s="12" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="13"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="12"/>
+      <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="1">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9" t="s">
+      <c r="H4" s="1">
+        <v>12</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11">
-        <v>1</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="11">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="11">
-        <v>3</v>
-      </c>
       <c r="H5" s="1">
-        <v>3</v>
-      </c>
-      <c r="I5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="1">
         <v>2</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="11">
-        <v>4</v>
-      </c>
       <c r="H6" s="1">
-        <v>4</v>
-      </c>
-      <c r="I6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="H1:I1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>